<commit_message>
Transfer updates to correct data folder
</commit_message>
<xml_diff>
--- a/data/Manuscripts.xlsx
+++ b/data/Manuscripts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Desktop/Microplastics in Drinking Water/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D8ACCA2-931B-F846-B5BA-516396E2E420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F074C58B-70C2-E945-8008-92D7E2C7FA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="11200" windowHeight="16880" xr2:uid="{C3B03CE3-0244-D74D-8763-9D44EA2F7D48}"/>
+    <workbookView xWindow="0" yWindow="6220" windowWidth="11200" windowHeight="16880" xr2:uid="{C3B03CE3-0244-D74D-8763-9D44EA2F7D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="206">
   <si>
     <t>DOI (DOI of manuscript being referenced)</t>
   </si>
@@ -320,13 +320,346 @@
   </si>
   <si>
     <t>Positive and negative lab controls</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pone.0236838</t>
+  </si>
+  <si>
+    <t>3 um; 0.2 um; 5 um; 0.22 um; 0.45 um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydrochloric acid; wet peroxide oxidation; acetic acid; </t>
+  </si>
+  <si>
+    <t>Stainless steel; membrane; anodisc; aluminum oxide</t>
+  </si>
+  <si>
+    <t>FTIR; Raman; m-FTIR; m-Raman</t>
+  </si>
+  <si>
+    <t>10.11001/jksww.2020.34.5.357</t>
+  </si>
+  <si>
+    <t>10.1016/j.scitotenv.2019.02.431</t>
+  </si>
+  <si>
+    <t>FTIR; Raman</t>
+  </si>
+  <si>
+    <t>10.1016/j.coesh.2018.12.001</t>
+  </si>
+  <si>
+    <t>10.1016/j.watres.2019.02.054</t>
+  </si>
+  <si>
+    <t>10.1016/j.cej.2020.128381</t>
+  </si>
+  <si>
+    <t>10.1016/j.jece.2020.104527</t>
+  </si>
+  <si>
+    <t>0.45-50 um</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>10.1016/j.chemosphere.2020.126612</t>
+  </si>
+  <si>
+    <t>trawl; glass filter; PTFE membrane filter; plankton net; nylon filter; sieve</t>
+  </si>
+  <si>
+    <t>1-500 um</t>
+  </si>
+  <si>
+    <t>ATR; FTIR; Raman</t>
+  </si>
+  <si>
+    <t>visual; stereomicroscope; microscope; SEM</t>
+  </si>
+  <si>
+    <t>10.1016/j.impact.2021.100302</t>
+  </si>
+  <si>
+    <t>calcium magnesium dissolusion; Fe H2O2; iron precipitates; HCl; H2O2;</t>
+  </si>
+  <si>
+    <t>polycarbonate; PTFE; Al3O3; Au coated polycarbonate; Al oxide</t>
+  </si>
+  <si>
+    <t>0.4 um; 5 um; 0.2 um; 0.22 um</t>
+  </si>
+  <si>
+    <t>FTIR; Raman; SEM-EDX</t>
+  </si>
+  <si>
+    <t>10.1007/s11783-021-1492-5</t>
+  </si>
+  <si>
+    <t>Literature review; drinking water treatment plants</t>
+  </si>
+  <si>
+    <t>10.1016/j.envres.2022.112855</t>
+  </si>
+  <si>
+    <t>Groundwater drinking water</t>
+  </si>
+  <si>
+    <t>H2O2</t>
+  </si>
+  <si>
+    <t>polycarbonate membrane</t>
+  </si>
+  <si>
+    <t>5 um</t>
+  </si>
+  <si>
+    <t>10.1021/acs.est.9b01517</t>
+  </si>
+  <si>
+    <t>Bottled water and tap water; food</t>
+  </si>
+  <si>
+    <t>10.1016/j.envpol.2021.117524</t>
+  </si>
+  <si>
+    <t>Drinking water</t>
+  </si>
+  <si>
+    <t>stainless steel</t>
+  </si>
+  <si>
+    <t>10.21203/rs.3.rs-242504/v1</t>
+  </si>
+  <si>
+    <t>Fe H2O2</t>
+  </si>
+  <si>
+    <t>10.1016/j.sciotenv.2020.143421</t>
+  </si>
+  <si>
+    <t>HCl</t>
+  </si>
+  <si>
+    <t>PC filter</t>
+  </si>
+  <si>
+    <t>1.2 um</t>
+  </si>
+  <si>
+    <t>EMCCD</t>
+  </si>
+  <si>
+    <t>10.1016/j.etap.2018.12.009</t>
+  </si>
+  <si>
+    <t>Reservoir water</t>
+  </si>
+  <si>
+    <t>978-82-414-0427-6</t>
+  </si>
+  <si>
+    <t>H2O2/H2SO4</t>
+  </si>
+  <si>
+    <t>Bottled water</t>
+  </si>
+  <si>
+    <t>10.1016/j.envpol.2020.114227</t>
+  </si>
+  <si>
+    <t>Public water fountains</t>
+  </si>
+  <si>
+    <t>nitrocellulose filter paper</t>
+  </si>
+  <si>
+    <t>0.22 um</t>
+  </si>
+  <si>
+    <t>Procedural blanks; filters analyzed before; cotton used; laminar flow hood used</t>
+  </si>
+  <si>
+    <t>10.1007/s11356-021-12467-y</t>
+  </si>
+  <si>
+    <t>100 um; 20 um; 10 um; 5 um</t>
+  </si>
+  <si>
+    <t>micro raman</t>
+  </si>
+  <si>
+    <t>Process blanks</t>
+  </si>
+  <si>
+    <t>10.3390/w12113115</t>
+  </si>
+  <si>
+    <t>7 um</t>
+  </si>
+  <si>
+    <t>Nile Red; flouresence microscopy</t>
+  </si>
+  <si>
+    <t>Referenced known particles under flouresence scope</t>
+  </si>
+  <si>
+    <t>10.3390/environments8120138</t>
+  </si>
+  <si>
+    <t>Drinking water type used by participants (study also included stool samples and food samples from participants)</t>
+  </si>
+  <si>
+    <t>Fenton's; HNO3</t>
+  </si>
+  <si>
+    <t>Cellulose nitrate-cellulose acetate</t>
+  </si>
+  <si>
+    <t>10.1016/j.cotox.2021.09.003</t>
+  </si>
+  <si>
+    <t>Review paper; Tap and bottled water</t>
+  </si>
+  <si>
+    <t>10.1016/j.jwpe.2020.101884</t>
+  </si>
+  <si>
+    <t>Gold plated polycarbonate</t>
+  </si>
+  <si>
+    <t>0.4 um</t>
+  </si>
+  <si>
+    <t>micro FTIR</t>
+  </si>
+  <si>
+    <t>laminar flow; cotton only in lab</t>
+  </si>
+  <si>
+    <t>10.1016/j.watres.2021.117417</t>
+  </si>
+  <si>
+    <t>cellulose acetate membrane</t>
+  </si>
+  <si>
+    <t>Zetasizer Nano ZS</t>
+  </si>
+  <si>
+    <t>10.1007/s11356-021-13220-1</t>
+  </si>
+  <si>
+    <t>stainless steel; membrane</t>
+  </si>
+  <si>
+    <t>3.5 mm; 1 mm; 300 um; 100 um; 20 um; 1 um</t>
+  </si>
+  <si>
+    <t>Steriomicroscopy; micro FTIR</t>
+  </si>
+  <si>
+    <t>3 procedural blanks; black filters washed with reagents analyzed</t>
+  </si>
+  <si>
+    <t>10.1016/j.cofs.2021.02.011</t>
+  </si>
+  <si>
+    <t>RM; micro FTIR; Nile Red; SEM</t>
+  </si>
+  <si>
+    <t>Procedural blanks</t>
+  </si>
+  <si>
+    <t>10.22630/PNIKS.2019.28.4.59</t>
+  </si>
+  <si>
+    <t>Fire hydrants; network water points; water holding tanks</t>
+  </si>
+  <si>
+    <t>cellulose</t>
+  </si>
+  <si>
+    <t>2-4 um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rose Bengal stain; visual; stereoscope </t>
+  </si>
+  <si>
+    <t>Review; Drinking water from treatment facilities</t>
+  </si>
+  <si>
+    <t>10.3390/app112110109</t>
+  </si>
+  <si>
+    <t>10.1016/j.jhazmat.2021.125347</t>
+  </si>
+  <si>
+    <t>glass microfiber</t>
+  </si>
+  <si>
+    <t>Procedural blanks; plastic equiptment minimized; cotton only worn in lab</t>
+  </si>
+  <si>
+    <t>10.1016/j.scitotenv.2020.140236</t>
+  </si>
+  <si>
+    <t>H2SO4</t>
+  </si>
+  <si>
+    <t>PTFE membrane; Al2O3</t>
+  </si>
+  <si>
+    <t>0.2 um</t>
+  </si>
+  <si>
+    <t>SEM; micro Raman</t>
+  </si>
+  <si>
+    <t>10.1016/j.chemosphere.2020.126493</t>
+  </si>
+  <si>
+    <t>Procedural blanks; laminar flow table</t>
+  </si>
+  <si>
+    <t>10.1016/j.scitotenv.2019.134520</t>
+  </si>
+  <si>
+    <t>0.5 um; 0.22 um</t>
+  </si>
+  <si>
+    <t>DWTP</t>
+  </si>
+  <si>
+    <t>Alumina filter</t>
+  </si>
+  <si>
+    <t>Plastic equiptment minimized</t>
+  </si>
+  <si>
+    <t>10.1007/s11356-021-13769-x</t>
+  </si>
+  <si>
+    <t>10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>Drinking water canal</t>
+  </si>
+  <si>
+    <t>10.1016/j.scitotenv.2022.154015</t>
+  </si>
+  <si>
+    <t>Al2O3</t>
+  </si>
+  <si>
+    <t>Procedural blanks; plastic equiptment minimized</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -338,6 +671,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -363,10 +703,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34ED786C-A5DE-5A46-A159-2F2BA9CB5F94}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="111" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1191,6 +1533,913 @@
         <v>94</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" t="s">
+        <v>112</v>
+      </c>
+      <c r="H27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" t="s">
+        <v>118</v>
+      </c>
+      <c r="G28" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" t="s">
+        <v>150</v>
+      </c>
+      <c r="G32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" t="s">
+        <v>149</v>
+      </c>
+      <c r="F38" t="s">
+        <v>150</v>
+      </c>
+      <c r="G38" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" t="s">
+        <v>153</v>
+      </c>
+      <c r="F39" t="s">
+        <v>154</v>
+      </c>
+      <c r="G39" t="s">
+        <v>155</v>
+      </c>
+      <c r="H39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F42" t="s">
+        <v>165</v>
+      </c>
+      <c r="G42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>167</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" t="s">
+        <v>169</v>
+      </c>
+      <c r="G43" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>171</v>
+      </c>
+      <c r="E44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F44" t="s">
+        <v>173</v>
+      </c>
+      <c r="G44" t="s">
+        <v>29</v>
+      </c>
+      <c r="H44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
+        <v>176</v>
+      </c>
+      <c r="G45" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>180</v>
+      </c>
+      <c r="E46" t="s">
+        <v>181</v>
+      </c>
+      <c r="F46" t="s">
+        <v>182</v>
+      </c>
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" t="s">
+        <v>186</v>
+      </c>
+      <c r="E48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F48" t="s">
+        <v>154</v>
+      </c>
+      <c r="G48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>188</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" t="s">
+        <v>189</v>
+      </c>
+      <c r="D49" t="s">
+        <v>190</v>
+      </c>
+      <c r="E49" t="s">
+        <v>191</v>
+      </c>
+      <c r="F49" t="s">
+        <v>192</v>
+      </c>
+      <c r="G49" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>193</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" t="s">
+        <v>191</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" t="s">
+        <v>190</v>
+      </c>
+      <c r="E51" t="s">
+        <v>196</v>
+      </c>
+      <c r="F51" t="s">
+        <v>192</v>
+      </c>
+      <c r="G51" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>200</v>
+      </c>
+      <c r="B52" t="s">
+        <v>197</v>
+      </c>
+      <c r="C52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52" t="s">
+        <v>198</v>
+      </c>
+      <c r="E52" t="s">
+        <v>191</v>
+      </c>
+      <c r="F52" t="s">
+        <v>57</v>
+      </c>
+      <c r="G52" t="s">
+        <v>29</v>
+      </c>
+      <c r="H52" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>201</v>
+      </c>
+      <c r="B53" t="s">
+        <v>202</v>
+      </c>
+      <c r="C53" t="s">
+        <v>123</v>
+      </c>
+      <c r="D53" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" t="s">
+        <v>204</v>
+      </c>
+      <c r="E54" t="s">
+        <v>191</v>
+      </c>
+      <c r="F54" t="s">
+        <v>165</v>
+      </c>
+      <c r="G54" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Move definitions from csv to README
</commit_message>
<xml_diff>
--- a/data/Manuscripts.xlsx
+++ b/data/Manuscripts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Desktop/Microplastics in Drinking Water/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Desktop/Microplastic_Data_Portal-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F074C58B-70C2-E945-8008-92D7E2C7FA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE47DFCA-6FD9-C24D-9ACA-5FF075151E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6220" windowWidth="11200" windowHeight="16880" xr2:uid="{C3B03CE3-0244-D74D-8763-9D44EA2F7D48}"/>
+    <workbookView xWindow="0" yWindow="3160" windowWidth="16600" windowHeight="16880" xr2:uid="{C3B03CE3-0244-D74D-8763-9D44EA2F7D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,36 +37,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="206">
   <si>
-    <t>DOI (DOI of manuscript being referenced)</t>
-  </si>
-  <si>
-    <t>Controls (type of controls used, if applicable)</t>
-  </si>
-  <si>
-    <t>Sample device and deployment methods (type and size of sample device used and how it was deployed)</t>
-  </si>
-  <si>
-    <t>Digestion (type of digestion used in preprocessing, if any)</t>
-  </si>
-  <si>
-    <t>Microplastic Identification Method (type(s) of identification used, e.g. visual, flourescent, SEM (scanning electron microscoscopy), light microscopy)</t>
-  </si>
-  <si>
-    <t>Spectral Analysis (type of spectral analysis used in study, if any, e.g. GC/MS, FTIR, Raman)</t>
-  </si>
-  <si>
     <t xml:space="preserve">10.1021/acs.est.9b06672 </t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Filtration (what type of filtration used)</t>
-  </si>
-  <si>
-    <t>Filter Size (size or sizes of filter(s))</t>
-  </si>
-  <si>
     <t>Raman; FTIR</t>
   </si>
   <si>
@@ -653,6 +629,30 @@
   </si>
   <si>
     <t>Procedural blanks; plastic equiptment minimized</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>Digestion</t>
+  </si>
+  <si>
+    <t>Filtration</t>
+  </si>
+  <si>
+    <t>Controls</t>
+  </si>
+  <si>
+    <t>Filter_Size</t>
+  </si>
+  <si>
+    <t>Microplastic_Identification_Method</t>
+  </si>
+  <si>
+    <t>Spectral_Analysis</t>
+  </si>
+  <si>
+    <t>Sample_device_and_deployment_methods</t>
   </si>
 </sst>
 </file>
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34ED786C-A5DE-5A46-A159-2F2BA9CB5F94}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="111" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="111" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,1401 +1043,1401 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>205</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>199</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>202</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>203</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>204</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
         <v>56</v>
       </c>
-      <c r="F13" t="s">
-        <v>64</v>
-      </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H15" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F16" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H18" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G20" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H20" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H23" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F26" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H26" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F27" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G27" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="H27" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D28" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E28" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F28" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G28" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H28" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D30" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E30" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H30" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H32" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F33" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G33" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H33" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E34" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F34" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H34" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G35" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H35" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F37" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G37" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H37" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E38" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F38" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G38" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H38" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E39" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F39" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G39" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H39" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G40" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H40" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B42" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E42" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F42" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="G42" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H42" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E43" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F43" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="G43" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E44" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F44" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="G44" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H44" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B45" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G45" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H45" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B46" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E46" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F46" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="G46" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B47" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D48" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F48" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G48" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H48" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D49" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E49" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F49" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G49" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H49" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E50" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F50" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G50" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H50" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D51" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E51" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F51" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G51" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H51" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B52" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D52" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="E52" t="s">
+        <v>183</v>
+      </c>
+      <c r="F52" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" t="s">
         <v>191</v>
-      </c>
-      <c r="F52" t="s">
-        <v>57</v>
-      </c>
-      <c r="G52" t="s">
-        <v>29</v>
-      </c>
-      <c r="H52" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B53" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D53" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E53" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D54" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E54" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F54" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="G54" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H54" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean manuscript/sample sheets, add polymer sheet
</commit_message>
<xml_diff>
--- a/data/Manuscripts.xlsx
+++ b/data/Manuscripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Desktop/Microplastic_Data_Portal-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE47DFCA-6FD9-C24D-9ACA-5FF075151E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3BC1BB-AC3D-E446-9F9F-EEC3962FA330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3160" windowWidth="16600" windowHeight="16880" xr2:uid="{C3B03CE3-0244-D74D-8763-9D44EA2F7D48}"/>
+    <workbookView xWindow="16820" yWindow="500" windowWidth="16600" windowHeight="16880" xr2:uid="{C3B03CE3-0244-D74D-8763-9D44EA2F7D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="206">
-  <si>
-    <t xml:space="preserve">10.1021/acs.est.9b06672 </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="190">
   <si>
     <t>N/A</t>
   </si>
@@ -46,9 +43,6 @@
     <t>Raman; FTIR</t>
   </si>
   <si>
-    <t>Gold coated polycarbonate; cellulose nitrate membrane; glass fiber filter; Whatman cellulose fiber</t>
-  </si>
-  <si>
     <t>10.1016/j.watres.2017.11.011</t>
   </si>
   <si>
@@ -94,12 +88,6 @@
     <t>Nile red; visual</t>
   </si>
   <si>
-    <t>Nile red; dissection microscope; SEM</t>
-  </si>
-  <si>
-    <t>0.45 mm; 5 um,;2.5 um; 1.5 um; 0.4 um; 0.2 um</t>
-  </si>
-  <si>
     <t>FTIR</t>
   </si>
   <si>
@@ -178,27 +166,12 @@
     <t>GCMS Pyrolysis</t>
   </si>
   <si>
-    <t>10.1016/j.chemosphere.2021.131881</t>
-  </si>
-  <si>
     <t>10 um</t>
   </si>
   <si>
     <t>Stereomicroscopy</t>
   </si>
   <si>
-    <t>Field blanks</t>
-  </si>
-  <si>
-    <t>Spiked tap water</t>
-  </si>
-  <si>
-    <t>10.1016/j.cej.2018.11.155</t>
-  </si>
-  <si>
-    <t>CCD camera to capture flocs</t>
-  </si>
-  <si>
     <t>10.1016/j.chemosphere.2021.132587</t>
   </si>
   <si>
@@ -226,9 +199,6 @@
     <t>HPLC grade water procedural blanks</t>
   </si>
   <si>
-    <t>10.1186/s43591-022-00030-6</t>
-  </si>
-  <si>
     <t>Literature review</t>
   </si>
   <si>
@@ -322,9 +292,6 @@
     <t>FTIR; Raman</t>
   </si>
   <si>
-    <t>10.1016/j.coesh.2018.12.001</t>
-  </si>
-  <si>
     <t>10.1016/j.watres.2019.02.054</t>
   </si>
   <si>
@@ -433,12 +400,6 @@
     <t>Reservoir water</t>
   </si>
   <si>
-    <t>978-82-414-0427-6</t>
-  </si>
-  <si>
-    <t>H2O2/H2SO4</t>
-  </si>
-  <si>
     <t>Bottled water</t>
   </si>
   <si>
@@ -512,15 +473,6 @@
   </si>
   <si>
     <t>laminar flow; cotton only in lab</t>
-  </si>
-  <si>
-    <t>10.1016/j.watres.2021.117417</t>
-  </si>
-  <si>
-    <t>cellulose acetate membrane</t>
-  </si>
-  <si>
-    <t>Zetasizer Nano ZS</t>
   </si>
   <si>
     <t>10.1007/s11356-021-13220-1</t>
@@ -703,12 +655,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34ED786C-A5DE-5A46-A159-2F2BA9CB5F94}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="111" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,160 +992,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" s="2"/>
+      <c r="A1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1206,33 +1156,33 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
@@ -1244,368 +1194,368 @@
         <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="H21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" t="s">
         <v>93</v>
       </c>
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>1</v>
-      </c>
       <c r="H22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1613,831 +1563,649 @@
         <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="H23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>96</v>
+      <c r="A24" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="D25" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="F25" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G25" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="G27" t="s">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>106</v>
+      <c r="A28" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="F28" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="H28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>111</v>
+      <c r="A29" t="s">
+        <v>114</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="E29" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="F29" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="G29" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H29" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D30" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="F31" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="G31" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>1</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="E32" t="s">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="F32" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="G32" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H32" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>123</v>
+      <c r="A33" t="s">
+        <v>131</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>133</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="H33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="E34" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="F34" t="s">
         <v>129</v>
       </c>
       <c r="G34" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H34" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>132</v>
+      <c r="A36" t="s">
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C36" t="s">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>1</v>
+        <v>142</v>
       </c>
       <c r="E36" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="F36" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="G36" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H36" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="F37" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="G37" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H37" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>152</v>
+      </c>
+      <c r="G38" t="s">
         <v>1</v>
       </c>
-      <c r="D38" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" t="s">
-        <v>141</v>
-      </c>
-      <c r="F38" t="s">
-        <v>142</v>
-      </c>
-      <c r="G38" t="s">
-        <v>6</v>
-      </c>
       <c r="H38" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>156</v>
       </c>
       <c r="E39" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="F39" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="G39" t="s">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="B40" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="D41" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="E41" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="F41" t="s">
-        <v>1</v>
+        <v>133</v>
       </c>
       <c r="G41" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H41" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B42" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>1</v>
+        <v>165</v>
       </c>
       <c r="D42" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="E42" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="F42" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="G42" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
       <c r="F43" t="s">
-        <v>161</v>
+        <v>16</v>
       </c>
       <c r="G43" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H43" t="s">
-        <v>1</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
+        <v>166</v>
+      </c>
+      <c r="E44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F44" t="s">
+        <v>168</v>
+      </c>
+      <c r="G44" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" t="s">
         <v>163</v>
-      </c>
-      <c r="E44" t="s">
-        <v>164</v>
-      </c>
-      <c r="F44" t="s">
-        <v>165</v>
-      </c>
-      <c r="G44" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" t="s">
         <v>167</v>
       </c>
-      <c r="B45" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>1</v>
-      </c>
       <c r="F45" t="s">
-        <v>168</v>
+        <v>44</v>
       </c>
       <c r="G45" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="H45" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C46" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="E46" t="s">
-        <v>173</v>
+        <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>174</v>
+        <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>1</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>176</v>
+      <c r="A47" t="s">
+        <v>179</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
+        <v>167</v>
       </c>
       <c r="F47" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="G47" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H47" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B48" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" t="s">
-        <v>115</v>
-      </c>
-      <c r="D48" t="s">
-        <v>178</v>
-      </c>
-      <c r="E48" t="s">
-        <v>45</v>
-      </c>
-      <c r="F48" t="s">
-        <v>146</v>
-      </c>
-      <c r="G48" t="s">
-        <v>21</v>
-      </c>
-      <c r="H48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>180</v>
-      </c>
-      <c r="B49" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" t="s">
         <v>181</v>
-      </c>
-      <c r="D49" t="s">
-        <v>182</v>
-      </c>
-      <c r="E49" t="s">
-        <v>183</v>
-      </c>
-      <c r="F49" t="s">
-        <v>184</v>
-      </c>
-      <c r="G49" t="s">
-        <v>6</v>
-      </c>
-      <c r="H49" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>185</v>
-      </c>
-      <c r="B50" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" t="s">
-        <v>183</v>
-      </c>
-      <c r="F50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50" t="s">
-        <v>6</v>
-      </c>
-      <c r="H50" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>187</v>
-      </c>
-      <c r="B51" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51" t="s">
-        <v>115</v>
-      </c>
-      <c r="D51" t="s">
-        <v>182</v>
-      </c>
-      <c r="E51" t="s">
-        <v>188</v>
-      </c>
-      <c r="F51" t="s">
-        <v>184</v>
-      </c>
-      <c r="G51" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>192</v>
-      </c>
-      <c r="B52" t="s">
-        <v>189</v>
-      </c>
-      <c r="C52" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" t="s">
-        <v>190</v>
-      </c>
-      <c r="E52" t="s">
-        <v>183</v>
-      </c>
-      <c r="F52" t="s">
-        <v>49</v>
-      </c>
-      <c r="G52" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>193</v>
-      </c>
-      <c r="B53" t="s">
-        <v>194</v>
-      </c>
-      <c r="C53" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" t="s">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>1</v>
-      </c>
-      <c r="G53" t="s">
-        <v>1</v>
-      </c>
-      <c r="H53" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>195</v>
-      </c>
-      <c r="B54" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" t="s">
-        <v>115</v>
-      </c>
-      <c r="D54" t="s">
-        <v>196</v>
-      </c>
-      <c r="E54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F54" t="s">
-        <v>157</v>
-      </c>
-      <c r="G54" t="s">
-        <v>21</v>
-      </c>
-      <c r="H54" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>